<commit_message>
Fix indentation TDDUIOrganization b6a7f0785228805e3e923f12642c0471636a2a18
</commit_message>
<xml_diff>
--- a/302-contenu-fhir---ajout-des-données-usager/ig/StructureDefinition-tddui-documentreference.xlsx
+++ b/302-contenu-fhir---ajout-des-données-usager/ig/StructureDefinition-tddui-documentreference.xlsx
@@ -60,7 +60,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2025-07-10T13:41:14+00:00</t>
+    <t>2025-07-10T14:59:37+00:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -854,7 +854,7 @@
     <t>DocumentReference.subject</t>
   </si>
   <si>
-    <t xml:space="preserve">Reference(https://hl7.fr/ig/fhir/core/StructureDefinition/fr-core-patient)
+    <t xml:space="preserve">Reference(https://interop.esante.gouv.fr/ig/fhir/tddui/StructureDefinition/fr-core-patient)
 </t>
   </si>
   <si>
@@ -1989,7 +1989,7 @@
     <col min="8" max="8" width="13.953125" customWidth="true" bestFit="true"/>
     <col min="9" max="9" width="11.3671875" customWidth="true" bestFit="true"/>
     <col min="10" max="10" width="20.703125" customWidth="true" bestFit="true"/>
-    <col min="11" max="11" width="66.81640625" customWidth="true" bestFit="true"/>
+    <col min="11" max="11" width="70.390625" customWidth="true" bestFit="true"/>
     <col min="12" max="12" width="100.703125" customWidth="true" bestFit="true"/>
     <col min="13" max="13" width="100.703125" customWidth="true" bestFit="true"/>
     <col min="14" max="14" width="100.703125" customWidth="true" bestFit="true"/>

</xml_diff>